<commit_message>
add functions to apply built-in styles
</commit_message>
<xml_diff>
--- a/border_test2.xlsx
+++ b/border_test2.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,13 +26,38 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="0"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.5999938962981048"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -56,16 +81,21 @@
       <bottom style="thick"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40 % - Accent1" xfId="1" builtinId="31" hidden="0"/>
+    <cellStyle name="Accent1" xfId="2" builtinId="29" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -679,132 +709,132 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>801</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>0.0336</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>0.05599999999999999</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <v>0.05599999999999999</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="n">
         <v>0.005</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="2" t="n">
         <v>801</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="3" t="n">
         <v>0.718</v>
       </c>
-      <c r="I2" s="2" t="n">
+      <c r="I2" s="3" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>802</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="n">
+      <c r="B3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="n">
         <v>802</v>
       </c>
-      <c r="H3" s="2" t="n">
+      <c r="H3" s="3" t="n">
         <v/>
       </c>
-      <c r="I3" s="2" t="n">
+      <c r="I3" s="3" t="n">
         <v/>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>803</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="n">
+      <c r="B4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="n">
         <v>803</v>
       </c>
-      <c r="H4" s="2" t="n">
+      <c r="H4" s="3" t="n">
         <v/>
       </c>
-      <c r="I4" s="2" t="n">
+      <c r="I4" s="3" t="n">
         <v/>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>804</v>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="n">
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="n">
         <v>804</v>
       </c>
-      <c r="H5" s="2" t="n">
+      <c r="H5" s="3" t="n">
         <v/>
       </c>
-      <c r="I5" s="2" t="n">
+      <c r="I5" s="3" t="n">
         <v/>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>805</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="3" t="n">
         <v>0.01</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="3" t="n">
         <v>0.05</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="3" t="n">
         <v>0.2</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="2" t="n">
         <v>805</v>
       </c>
-      <c r="H6" s="2" t="n">
+      <c r="H6" s="3" t="n">
         <v>0.24</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="I6" s="3" t="n">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add more functions - 4/26/23 version
</commit_message>
<xml_diff>
--- a/border_test2.xlsx
+++ b/border_test2.xlsx
@@ -673,6 +673,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <cols>
+    <col width="15.6" customWidth="1" min="2" max="2"/>
+    <col width="15.6" customWidth="1" min="3" max="3"/>
+    <col width="15.6" customWidth="1" min="4" max="4"/>
+    <col width="15.6" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">

</xml_diff>